<commit_message>
Update lenh cho bep hai san 179
</commit_message>
<xml_diff>
--- a/CMS.Web/Modules/Sails/Admin/ExportTemplates/lenh_cho_bep_2.xlsx
+++ b/CMS.Web/Modules/Sails/Admin/ExportTemplates/lenh_cho_bep_2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Project\haisan179\CMS.Web\Modules\Sails\Admin\ExportTemplates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96658E6-6DA7-4F6B-9E00-3B171D09F670}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{521A92CE-EEF8-438B-A7CE-60D7EEF63D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4200" yWindow="4200" windowWidth="17280" windowHeight="8970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="1" r:id="rId1"/>
@@ -50,12 +50,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="D2" authorId="0" shapeId="0" xr:uid="{52E56758-6434-41B7-8152-1678E986EDAC}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Nguyen :</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Số luongj khách</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="5">
   <si>
     <t>Du Lich Binh An</t>
   </si>
@@ -151,7 +175,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -179,6 +203,19 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -205,10 +242,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -549,36 +586,49 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="27.85546875" customWidth="1"/>
+    <col min="3" max="3" width="39.140625" customWidth="1"/>
+    <col min="4" max="4" width="27.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:2" ht="51" customHeight="1" x14ac:dyDescent="0.6">
+    <row r="1" spans="1:4" ht="31.5" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:4" ht="51" customHeight="1" x14ac:dyDescent="0.6">
       <c r="A2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
+      <c r="C2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="3" spans="1:2" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+    <row r="3" spans="1:4" ht="409.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="6"/>
+      <c r="B3" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="5"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A3:B3"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="landscape" r:id="rId1"/>

</xml_diff>